<commit_message>
Updated Wallet Add Transaction E2E
</commit_message>
<xml_diff>
--- a/e2e/wallets/wallet-add-transaction - formulas.xlsx
+++ b/e2e/wallets/wallet-add-transaction - formulas.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\stock-portfolio-tracker\e2e\wallets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4E6A10CA-AB79-4EC1-A73B-40488735CAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC256CA3-4218-46D3-B73F-29C9B34E9F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="8910" windowWidth="48705" windowHeight="13035" xr2:uid="{9097CB89-00AB-4C99-8F72-09B669EC784E}"/>
+    <workbookView xWindow="4035" yWindow="7965" windowWidth="48705" windowHeight="13035" xr2:uid="{098A0282-4D56-4627-9BA7-FE6DDAC8294F}"/>
   </bookViews>
   <sheets>
-    <sheet name="wallet-add-transaction - formul" sheetId="1" r:id="rId1"/>
+    <sheet name="wallet-add-transaction" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,9 +68,6 @@
     <t>plr</t>
   </si>
   <si>
-    <t>swingHoldRatio</t>
-  </si>
-  <si>
     <t>lbd</t>
   </si>
   <si>
@@ -103,6 +113,9 @@
     <t>stockSwingHoldRatio</t>
   </si>
   <si>
+    <t>stockCommission</t>
+  </si>
+  <si>
     <t>SplitBuyInitial</t>
   </si>
   <si>
@@ -148,13 +161,17 @@
     <t>AnotherSplitBuy</t>
   </si>
   <si>
-    <t>LBD</t>
+    <t>_5DD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,10 +649,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1010,41 +1029,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D37946-C4E2-41A8-800B-C79B8A44BE73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30F172C-A8FF-4EB3-844D-D842EBA3A643}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1072,7 +1091,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -1081,25 +1100,25 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" t="s">
@@ -1134,7 +1153,7 @@
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>45792</v>
       </c>
       <c r="C2" s="1">
@@ -1150,14 +1169,14 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H2">
         <v>200</v>
       </c>
       <c r="I2" s="2">
         <f>H2/G2</f>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -1165,61 +1184,67 @@
       <c r="K2">
         <v>2</v>
       </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
-      <c r="M2">
-        <f>G2-(G2*J2%)</f>
-        <v>9.5</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
+      <c r="L2" s="3">
+        <f>(G2-(G2*J2%))/(1+(AA2/100))</f>
+        <v>94.905094905094913</v>
+      </c>
+      <c r="M2" s="2">
+        <f>G2</f>
         <v>100</v>
       </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <v>10</v>
-      </c>
-      <c r="R2">
+      <c r="N2" s="2">
+        <f>Z2/100*H2</f>
+        <v>140</v>
+      </c>
+      <c r="O2" s="2">
+        <f>Z2/100*I2</f>
+        <v>1.4</v>
+      </c>
+      <c r="P2" s="2">
+        <f>G2</f>
         <v>100</v>
       </c>
-      <c r="S2">
-        <v>10</v>
+      <c r="Q2" s="2">
+        <f>(100-Z2)/100*H2</f>
+        <v>60</v>
+      </c>
+      <c r="R2" s="2">
+        <f>(100-Z2)/100*I2</f>
+        <v>0.6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>31</v>
       </c>
       <c r="T2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" t="s">
         <v>34</v>
       </c>
+      <c r="W2">
+        <v>5</v>
+      </c>
       <c r="X2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y2">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="Z2">
-        <v>600</v>
+        <v>70</v>
       </c>
       <c r="AA2">
-        <v>50</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>45793</v>
       </c>
       <c r="C3" s="1">
@@ -1235,14 +1260,14 @@
         <v>37</v>
       </c>
       <c r="G3">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="H3">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3:I5" si="0">H3/G3</f>
-        <v>20</v>
+        <v>1.6</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -1250,61 +1275,66 @@
       <c r="K3">
         <v>2</v>
       </c>
-      <c r="L3">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M5" si="1">G3-(G3*J3%)</f>
-        <v>23.75</v>
-      </c>
-      <c r="N3">
-        <v>25</v>
-      </c>
-      <c r="O3">
-        <v>500</v>
-      </c>
-      <c r="P3">
-        <v>20</v>
-      </c>
-      <c r="Q3">
+      <c r="L3" s="3">
+        <f>(G3-(G3*J3%))/(1+(AA3/100))</f>
+        <v>236.78963110667999</v>
+      </c>
+      <c r="M3" s="2">
+        <f>G3</f>
+        <v>250</v>
+      </c>
+      <c r="N3" s="2">
+        <f>Z3/100*H3</f>
+        <v>400</v>
+      </c>
+      <c r="O3" s="2">
+        <f>Z3/100*I3</f>
+        <v>1.6</v>
+      </c>
+      <c r="P3" s="2">
         <v>0</v>
       </c>
-      <c r="R3">
+      <c r="Q3" s="2">
+        <f>(100-Z3)/100*H3</f>
         <v>0</v>
       </c>
-      <c r="S3">
+      <c r="R3" s="2">
+        <f>(100-Z3)/100*I3</f>
         <v>0</v>
       </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
       <c r="T3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V3" t="s">
-        <v>33</v>
-      </c>
-      <c r="W3" t="s">
         <v>34</v>
       </c>
+      <c r="W3">
+        <v>5</v>
+      </c>
       <c r="X3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y3">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="Z3">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="AA3">
-        <v>50</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>45794</v>
       </c>
       <c r="C4" s="1">
@@ -1320,14 +1350,14 @@
         <v>40</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>900</v>
       </c>
       <c r="H4">
         <v>350</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="J4">
         <v>5</v>
@@ -1335,61 +1365,67 @@
       <c r="K4">
         <v>2</v>
       </c>
-      <c r="L4">
-        <v>50</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="1"/>
-        <v>6.65</v>
-      </c>
-      <c r="N4">
+      <c r="L4" s="3">
+        <f>(G4-(G4*J4%))/(1+(AA4/100))</f>
+        <v>846.53465346534654</v>
+      </c>
+      <c r="M4" s="2">
+        <f>G4</f>
+        <v>900</v>
+      </c>
+      <c r="N4" s="2">
+        <f>Z4/100*H4</f>
         <v>0</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
+        <f>Z4/100*I4</f>
         <v>0</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
+        <f>G4</f>
+        <v>900</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>(100-Z4)/100*H4</f>
+        <v>350</v>
+      </c>
+      <c r="R4" s="3">
+        <f>(100-Z4)/100*I4</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="S4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
+        <v>600</v>
+      </c>
+      <c r="Z4">
         <v>0</v>
       </c>
-      <c r="Q4">
-        <v>7</v>
-      </c>
-      <c r="R4">
-        <v>350</v>
-      </c>
-      <c r="S4">
-        <v>50</v>
-      </c>
-      <c r="T4" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" t="s">
-        <v>33</v>
-      </c>
-      <c r="W4" t="s">
-        <v>34</v>
-      </c>
-      <c r="X4">
-        <v>5</v>
-      </c>
-      <c r="Y4">
-        <v>2</v>
-      </c>
-      <c r="Z4">
-        <v>600</v>
-      </c>
       <c r="AA4">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>45795</v>
       </c>
       <c r="C5" s="1">
@@ -1405,14 +1441,14 @@
         <v>42</v>
       </c>
       <c r="G5">
+        <v>500.34</v>
+      </c>
+      <c r="H5">
         <v>100</v>
-      </c>
-      <c r="H5">
-        <v>1000</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.19986409241715633</v>
       </c>
       <c r="J5">
         <v>5</v>
@@ -1420,57 +1456,64 @@
       <c r="K5">
         <v>2</v>
       </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="N5">
-        <v>100</v>
-      </c>
-      <c r="O5">
-        <v>500</v>
-      </c>
-      <c r="P5">
+      <c r="L5" s="3">
+        <f>(G5-(G5*J5%))/(1+(AA5/100))</f>
+        <v>475.32299999999998</v>
+      </c>
+      <c r="M5" s="2">
+        <f>G5</f>
+        <v>500.34</v>
+      </c>
+      <c r="N5" s="2">
+        <f>Z5/100*H5</f>
+        <v>10</v>
+      </c>
+      <c r="O5" s="3">
+        <f>Z5/100*I5</f>
+        <v>1.9986409241715634E-2</v>
+      </c>
+      <c r="P5" s="2">
+        <f>G5</f>
+        <v>500.34</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>(100-Z5)/100*H5</f>
+        <v>90</v>
+      </c>
+      <c r="R5" s="3">
+        <f>(100-Z5)/100*I5</f>
+        <v>0.1798776831754407</v>
+      </c>
+      <c r="S5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5">
         <v>5</v>
       </c>
-      <c r="Q5">
-        <v>100</v>
-      </c>
-      <c r="R5">
-        <v>500</v>
-      </c>
-      <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V5" t="s">
-        <v>33</v>
-      </c>
-      <c r="W5" t="s">
-        <v>34</v>
-      </c>
       <c r="X5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Y5">
-        <v>2</v>
+        <v>600</v>
       </c>
       <c r="Z5">
-        <v>600</v>
+        <v>10</v>
       </c>
       <c r="AA5">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>